<commit_message>
Consoidated TestNg and Notification disabling
</commit_message>
<xml_diff>
--- a/data/CreateCMS.xlsx
+++ b/data/CreateCMS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>CMSName</t>
   </si>
@@ -30,28 +30,40 @@
     <t>Language</t>
   </si>
   <si>
-    <t>Test 2</t>
-  </si>
-  <si>
     <t>Star</t>
   </si>
   <si>
     <t>English (United States)</t>
   </si>
   <si>
-    <t>CM 145</t>
-  </si>
-  <si>
-    <t>CM 146</t>
-  </si>
-  <si>
-    <t>Test 3</t>
-  </si>
-  <si>
     <t>German</t>
   </si>
   <si>
     <t>Sportz</t>
+  </si>
+  <si>
+    <t>CM 1515</t>
+  </si>
+  <si>
+    <t>CM 1516</t>
+  </si>
+  <si>
+    <t>CM 1517</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Zee</t>
+  </si>
+  <si>
+    <t>Test 1517</t>
+  </si>
+  <si>
+    <t>Test 1516</t>
+  </si>
+  <si>
+    <t>Test 1515</t>
   </si>
 </sst>
 </file>
@@ -383,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -413,30 +425,44 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>